<commit_message>
rough code for simulating pop dy and obs model
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Fleet_Selex_Sim/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A66A40A-932D-4C4E-A38F-9529F9D638F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7B19A5-7B0C-6A48-90BA-B0EB019C3778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,7 +649,7 @@
         <v>30</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -1565,7 +1565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding options to switch between length and age-based selectivity in om and em
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5C2FB8-1B47-CA4A-B8D9-694650229CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E22E39D-E11B-0A45-B342-6A7E0F8C7849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30040" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>Par</t>
   </si>
@@ -114,9 +114,6 @@
     <t>beta</t>
   </si>
   <si>
-    <t>alpha</t>
-  </si>
-  <si>
     <t>vonB_sd</t>
   </si>
   <si>
@@ -147,15 +144,9 @@
     <t>fish_len_midpoint</t>
   </si>
   <si>
-    <t>Midpoint of logistic selectivity</t>
-  </si>
-  <si>
     <t>srv_len_slope</t>
   </si>
   <si>
-    <t>slope of logistic selectivity</t>
-  </si>
-  <si>
     <t>srv_len_midpoint</t>
   </si>
   <si>
@@ -163,6 +154,45 @@
   </si>
   <si>
     <t>Number of years</t>
+  </si>
+  <si>
+    <t>fish_age_slope_f</t>
+  </si>
+  <si>
+    <t>fish_age_slope_m</t>
+  </si>
+  <si>
+    <t>fish_age_midpoint_f</t>
+  </si>
+  <si>
+    <t>fish_age_midpoint_m</t>
+  </si>
+  <si>
+    <t>srv_age_slope_f</t>
+  </si>
+  <si>
+    <t>srv_age_slope_m</t>
+  </si>
+  <si>
+    <t>srv_age_midpoint_f</t>
+  </si>
+  <si>
+    <t>srv_age_midpoint_m</t>
+  </si>
+  <si>
+    <t>slope of logistic selectivity (age-based)</t>
+  </si>
+  <si>
+    <t>Midpoint of logistic selectivity (age-based)</t>
+  </si>
+  <si>
+    <t>slope of logistic selectivity (length-based)</t>
+  </si>
+  <si>
+    <t>Midpoint of logistic selectivity (length-based)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha </t>
   </si>
 </sst>
 </file>
@@ -537,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -562,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -600,13 +630,13 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -616,10 +646,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963305BC-AF74-9C4D-830B-80A9AEA5B8F2}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -637,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -645,7 +675,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -653,7 +683,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -661,7 +691,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -669,7 +699,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -677,7 +707,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -685,7 +715,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -693,7 +723,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -701,7 +731,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -709,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -717,7 +747,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -725,7 +755,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -733,7 +763,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -741,7 +771,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -749,7 +779,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -757,7 +787,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -765,7 +795,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -773,7 +803,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -781,7 +811,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -789,7 +819,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -797,7 +827,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -805,7 +835,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -813,7 +843,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -821,7 +851,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -829,7 +859,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -837,7 +867,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -845,7 +875,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -853,7 +883,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -861,7 +891,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -869,7 +899,12 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>99</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1148,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1214,10 +1249,10 @@
         <v>1.004104E-5</v>
       </c>
       <c r="B6" s="2">
-        <v>9.45386E-6</v>
+        <v>9.4499999999999993E-6</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1228,18 +1263,18 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1338,10 +1373,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A22188-D96C-2C44-BBAD-F7C7BF93AA5F}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1362,46 +1397,134 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3">
-        <v>63.5</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="3">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
+      <c r="B6">
+        <v>0.7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>0.9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>0.45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>0.35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1414,7 +1537,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1465,35 +1588,35 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>0.5</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>0.125</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
addding in fmsy reference points
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E22E39D-E11B-0A45-B342-6A7E0F8C7849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66464830-6368-DB4D-8EAC-1C147D17D86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1376,7 +1376,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1602,7 +1602,7 @@
         <v>28</v>
       </c>
       <c r="B6">
-        <v>7.4999999999999997E-2</v>
+        <v>0.108</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
adding in fmsy c alculations in OM
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66464830-6368-DB4D-8EAC-1C147D17D86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843DB962-DDB2-BC4E-80BD-09005FAD1807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
functions for plots, and fixing r0 bug in bmsy
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843DB962-DDB2-BC4E-80BD-09005FAD1807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB71E68A-73F0-C446-A103-5B9A6AB0148A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -567,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
+    <sheetView zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1183,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1205,7 +1205,7 @@
         <v>0.17</v>
       </c>
       <c r="B2">
-        <v>0.27</v>
+        <v>0.2</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -1213,10 +1213,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>81.2</v>
+        <v>95</v>
       </c>
       <c r="B3">
-        <v>67.900000000000006</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -1376,7 +1376,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
getting BMSY and FMSY right
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB71E68A-73F0-C446-A103-5B9A6AB0148A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF6A4AE-5B62-AE4E-9792-798D941B7C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1183,7 +1183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1537,7 +1537,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1580,7 +1580,7 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
further vlaidating model and making simulation faster
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF6A4AE-5B62-AE4E-9792-798D941B7C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A279E1-7F0C-E046-A95C-E63E444D057D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
adding options to fit sex ratios
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D221A898-6A31-3346-9BF2-C2CCAB61EBAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FDB766-CAC8-E14C-8D7C-4CB8545C2F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -633,7 +633,7 @@
         <v>36</v>
       </c>
       <c r="B6">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -1183,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1202,10 +1202,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="B2">
-        <v>0.1275</v>
+        <v>0.2</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -1216,7 +1216,7 @@
         <v>95</v>
       </c>
       <c r="B3">
-        <v>80.75</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -1536,7 +1536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1613,7 +1613,7 @@
         <v>30</v>
       </c>
       <c r="B7">
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
adding in sloping harvest control rule
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FDB766-CAC8-E14C-8D7C-4CB8545C2F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD75B9CC-E27B-EA49-90A0-0C330009B00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -567,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -633,7 +633,7 @@
         <v>36</v>
       </c>
       <c r="B6">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -1183,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E772079-C832-FD41-B10C-458366B30A38}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1537,7 +1537,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
fixing some sex ratio stuff
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD75B9CC-E27B-EA49-90A0-0C330009B00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93864FB-32B9-9A4D-BB9D-40F15079AB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -567,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
+    <sheetView zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1536,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1591,7 +1591,7 @@
         <v>26</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
adding in sex ratio for len comps
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93864FB-32B9-9A4D-BB9D-40F15079AB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB195A6-0AAA-BD49-B429-2E509C0339D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="5" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -633,7 +633,7 @@
         <v>36</v>
       </c>
       <c r="B6">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -1536,7 +1536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixing stuff and set up simulations
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103FE6B0-FAF6-9E43-9F9D-F1569011B235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2375C1C9-5473-0342-8BFB-8A127E19F1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>Par</t>
   </si>
@@ -118,12 +118,6 @@
   </si>
   <si>
     <t>wl_sd</t>
-  </si>
-  <si>
-    <t>sexRatio</t>
-  </si>
-  <si>
-    <t>Sex Ratio</t>
   </si>
   <si>
     <t>M_Female</t>
@@ -568,7 +562,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -592,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -630,13 +624,13 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -916,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F627ED8-0584-9F44-A42E-8F099BFE09BF}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="T1" workbookViewId="0">
       <selection activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
@@ -1184,7 +1178,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1205,7 +1199,7 @@
         <v>0.17</v>
       </c>
       <c r="B2">
-        <v>0.2</v>
+        <v>0.23</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -1213,10 +1207,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>95</v>
+        <v>81.2</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>66.5</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -1224,10 +1218,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>-2.98</v>
+        <v>-3.28</v>
       </c>
       <c r="B4">
-        <v>-2.41</v>
+        <v>-3.28</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -1249,10 +1243,10 @@
         <v>1.004104E-5</v>
       </c>
       <c r="B6" s="2">
-        <v>9.4499999999999993E-6</v>
+        <v>1.004104E-5</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1397,134 +1391,134 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0.35</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>0.35</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3">
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>0.7</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>0.9</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10">
         <v>0.45</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B11">
         <v>0.35</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1534,10 +1528,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28C32CEA-4D0B-9142-97E4-4A6BC1927971}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1591,7 +1585,7 @@
         <v>26</v>
       </c>
       <c r="B5">
-        <v>0.7</v>
+        <v>0.108</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
@@ -1606,17 +1600,6 @@
       </c>
       <c r="C6" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7">
-        <v>0.15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update EM to fit SR by year only and re-runs
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2375C1C9-5473-0342-8BFB-8A127E19F1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3B4B96-B7C1-4242-900C-7A2602F024C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
+    <sheetView zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -643,7 +643,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1369,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A22188-D96C-2C44-BBAD-F7C7BF93AA5F}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1405,7 +1405,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>57.5</v>
       </c>
       <c r="C3" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
updating vonB sd paramterization
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3B4B96-B7C1-4242-900C-7A2602F024C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD45056-2F1C-3149-87F1-9CA32AD008BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Par</t>
   </si>
@@ -114,9 +114,6 @@
     <t>beta</t>
   </si>
   <si>
-    <t>vonB_sd</t>
-  </si>
-  <si>
     <t>wl_sd</t>
   </si>
   <si>
@@ -187,6 +184,12 @@
   </si>
   <si>
     <t xml:space="preserve">alpha </t>
+  </si>
+  <si>
+    <t>vonB_sd_2</t>
+  </si>
+  <si>
+    <t>vonB_sd_1</t>
   </si>
 </sst>
 </file>
@@ -561,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC65A0B-C947-E946-A19B-823C994D6250}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -624,13 +627,13 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -640,10 +643,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963305BC-AF74-9C4D-830B-80A9AEA5B8F2}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -894,11 +897,6 @@
       </c>
       <c r="B31">
         <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="B32">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1178,7 +1176,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1246,33 +1244,42 @@
         <v>1.004104E-5</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4">
+      <c r="A9">
+        <v>0.2</v>
+      </c>
+      <c r="B9">
+        <v>0.2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4">
@@ -1369,7 +1376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A22188-D96C-2C44-BBAD-F7C7BF93AA5F}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -1391,134 +1398,134 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>0.35</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>57.5</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>0.35</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3">
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>0.7</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>0.9</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>0.45</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>0.35</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1582,24 +1589,24 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>0.108</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>0.108</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code updte cfor comps
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69722E93-D991-0A43-A14C-3BD6C484632C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED18CF0-E9D5-E24B-9608-DB44CA99230F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Controls" sheetId="1" r:id="rId1"/>
@@ -565,7 +565,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1377,7 +1377,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1401,7 +1401,7 @@
         <v>29</v>
       </c>
       <c r="B2">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -1412,7 +1412,7 @@
         <v>30</v>
       </c>
       <c r="B3">
-        <v>57.5</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -1423,7 +1423,7 @@
         <v>31</v>
       </c>
       <c r="B4">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
       <c r="C4" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
update sex str runs
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED18CF0-E9D5-E24B-9608-DB44CA99230F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10EF1DD-4BFF-5C49-A6A6-43D724F34AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -565,7 +565,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="239" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1401,7 +1401,7 @@
         <v>29</v>
       </c>
       <c r="B2">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -1412,7 +1412,7 @@
         <v>30</v>
       </c>
       <c r="B3">
-        <v>60</v>
+        <v>62.5</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
@@ -1423,7 +1423,7 @@
         <v>31</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="C4" t="s">
         <v>45</v>
@@ -1434,7 +1434,7 @@
         <v>32</v>
       </c>
       <c r="B5" s="3">
-        <v>50</v>
+        <v>52.5</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
adding experiment 3 and toying with some code
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10EF1DD-4BFF-5C49-A6A6-43D724F34AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141865A5-1104-CD41-9CB4-E0C22F2415FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -266,9 +266,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -306,7 +306,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -412,7 +412,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -554,7 +554,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>

<commit_message>
update code and fix bug on simulating CAL data
</commit_message>
<xml_diff>
--- a/input/Sablefish_Inputs.xlsx
+++ b/input/Sablefish_Inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewcheng/Desktop/UAF Thesis/Sex_Strc_Sim/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3AA89F-18AF-1443-A3B1-3212E3CE5DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BF1AA3-E5C5-8C4C-B5BE-F5692B8EC098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4080" yWindow="1600" windowWidth="30240" windowHeight="18880" xr2:uid="{CA348ABE-781E-D04E-90A2-7352F3084E81}"/>
   </bookViews>
@@ -266,9 +266,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -306,7 +306,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -412,7 +412,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -554,7 +554,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -589,7 +589,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>750</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>